<commit_message>
with material theme and hamburger menu
</commit_message>
<xml_diff>
--- a/Documents/FeatureList/FeatureList.xlsx
+++ b/Documents/FeatureList/FeatureList.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FeatureList!$D$5:$G$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FeatureList!$D$5:$G$32</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="60">
   <si>
     <t>Feature ID</t>
   </si>
@@ -126,6 +126,15 @@
     <t>EON/FE/ID-24</t>
   </si>
   <si>
+    <t>EON/FE/ID-25</t>
+  </si>
+  <si>
+    <t>EON/FE/ID-26</t>
+  </si>
+  <si>
+    <t>EON/FE/ID-27</t>
+  </si>
+  <si>
     <t>As a Store manager, I should be able to manage the user profiles of the stores which am supervising</t>
   </si>
   <si>
@@ -190,16 +199,13 @@
   </si>
   <si>
     <t>As a Customer, I should be able to get receipt when I pays at pump</t>
-  </si>
-  <si>
-    <t>n</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,12 +220,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Wingdings"/>
-      <charset val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -441,6 +441,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -487,7 +488,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,357 +787,362 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D4:H29"/>
+  <dimension ref="D4:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
     <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="79.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="79.42578125" style="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:8" ht="15.75" thickBot="1"/>
-    <row r="5" spans="4:8">
+    <row r="4" spans="4:7" ht="15.75" thickBot="1"/>
+    <row r="5" spans="4:7">
       <c r="D5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="15" t="s">
+      <c r="E5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="16" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="4:8" ht="30">
+    <row r="6" spans="4:7" ht="30">
       <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="8" t="s">
+      <c r="E6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="4:8" ht="30">
+    <row r="7" spans="4:7" ht="30">
       <c r="D7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>49</v>
+      <c r="E7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="4:8" ht="30">
+    <row r="8" spans="4:7" ht="30">
       <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>50</v>
+      <c r="E8" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="4:8">
+    <row r="9" spans="4:7">
       <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="8" t="s">
+      <c r="E9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="4:8">
+    <row r="10" spans="4:7">
       <c r="D10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>51</v>
+      <c r="E10" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="4:8" ht="30">
+    <row r="11" spans="4:7" ht="30">
       <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="8" t="s">
+      <c r="E11" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="4:8">
+    </row>
+    <row r="12" spans="4:7">
       <c r="D12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="8" t="s">
+      <c r="E12" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="4:8" ht="30">
+    </row>
+    <row r="13" spans="4:7" ht="30">
       <c r="D13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>52</v>
+      <c r="E13" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="4:8">
+    </row>
+    <row r="14" spans="4:7">
       <c r="D14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>53</v>
+      <c r="E14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="G14" s="4"/>
-      <c r="H14" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="4:8">
+    </row>
+    <row r="15" spans="4:7">
       <c r="D15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="8" t="s">
+      <c r="E15" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G15" s="4"/>
-      <c r="H15" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="4:8" ht="30">
+    </row>
+    <row r="16" spans="4:7" ht="30">
       <c r="D16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>23</v>
+      <c r="F16" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="G16" s="4"/>
-      <c r="H16" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="4:8">
+    </row>
+    <row r="17" spans="4:7">
       <c r="D17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="11" t="s">
-        <v>24</v>
+      <c r="F17" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="G17" s="4"/>
-      <c r="H17" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="4:8" ht="30">
+    </row>
+    <row r="18" spans="4:7">
       <c r="D18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>54</v>
+      <c r="E18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="G18" s="4"/>
-      <c r="H18" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="4:8" ht="30">
+    </row>
+    <row r="19" spans="4:7" ht="30">
       <c r="D19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>28</v>
+      <c r="E19" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="G19" s="4"/>
-      <c r="H19" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="4:8" ht="30">
+    </row>
+    <row r="20" spans="4:7">
       <c r="D20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>35</v>
+      <c r="E20" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="G20" s="4"/>
-      <c r="H20" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="4:8">
+    </row>
+    <row r="21" spans="4:7" ht="30">
       <c r="D21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="16" t="s">
+      <c r="E21" s="13" t="s">
         <v>42</v>
       </c>
+      <c r="F21" s="14" t="s">
+        <v>57</v>
+      </c>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="4:8">
+    <row r="22" spans="4:7" ht="30">
       <c r="D22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>43</v>
+      <c r="E22" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="4:8" ht="30">
+    <row r="23" spans="4:7" ht="30">
       <c r="D23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>44</v>
+      <c r="E23" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>38</v>
       </c>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="4:8" ht="30">
+    <row r="24" spans="4:7">
       <c r="D24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>55</v>
+      <c r="E24" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>45</v>
       </c>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="4:8" ht="30">
+    <row r="25" spans="4:7">
       <c r="D25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>48</v>
+      <c r="E25" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>46</v>
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="4:8">
+    <row r="26" spans="4:7" ht="30">
       <c r="D26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="10" t="s">
         <v>40</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="4:8">
+    <row r="27" spans="4:7" ht="30">
       <c r="D27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="10" t="s">
         <v>40</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="4:8">
+    <row r="28" spans="4:7" ht="30">
       <c r="D28" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="E28" s="10" t="s">
         <v>40</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="4:8" ht="15.75" thickBot="1">
+    <row r="29" spans="4:7">
       <c r="D29" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F29" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="G29" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="4:7">
+      <c r="D30" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="4:7">
+      <c r="D31" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="4:7" ht="15.75" thickBot="1">
+      <c r="D32" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="G32" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="D5:G29"/>
+  <autoFilter ref="D5:G32"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1157,40 +1162,40 @@
   <sheetData>
     <row r="4" spans="3:4" ht="15.75" thickBot="1"/>
     <row r="5" spans="3:4">
-      <c r="C5" s="19"/>
-      <c r="D5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
     </row>
     <row r="6" spans="3:4">
-      <c r="C6" s="21"/>
-      <c r="D6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="23"/>
     </row>
     <row r="7" spans="3:4">
-      <c r="C7" s="21"/>
-      <c r="D7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="23"/>
     </row>
     <row r="8" spans="3:4">
-      <c r="C8" s="21"/>
-      <c r="D8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="23"/>
     </row>
     <row r="9" spans="3:4">
-      <c r="C9" s="21"/>
-      <c r="D9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="23"/>
     </row>
     <row r="10" spans="3:4">
-      <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="23"/>
     </row>
     <row r="11" spans="3:4">
-      <c r="C11" s="21"/>
-      <c r="D11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="23"/>
     </row>
     <row r="12" spans="3:4">
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="23"/>
     </row>
     <row r="13" spans="3:4" ht="15.75" thickBot="1">
-      <c r="C13" s="23"/>
-      <c r="D13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>